<commit_message>
updated chromedriver and done changes in BaseClass
</commit_message>
<xml_diff>
--- a/com.crm.SDET35(copy)/src/test/resources/PurchaseOrder.xlsx
+++ b/com.crm.SDET35(copy)/src/test/resources/PurchaseOrder.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15690" windowHeight="3840"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15765" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="PurchaseOrder" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
@@ -422,7 +423,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>